<commit_message>
Add solution(bug-report) task 1
</commit_message>
<xml_diff>
--- a/Bug-reports/Bug-report_1.xlsx
+++ b/Bug-reports/Bug-report_1.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Task1" sheetId="1" r:id="rId1"/>
+    <sheet name="Task" sheetId="1" r:id="rId1"/>
+    <sheet name="Bug-report" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <r>
       <rPr>
@@ -69,12 +70,93 @@
       <t xml:space="preserve"> www.testmovies.com</t>
     </r>
   </si>
+  <si>
+    <t>BUG 001</t>
+  </si>
+  <si>
+    <t>001 [movie search] invalid movie search result when the user searches for a non-existent movie</t>
+  </si>
+  <si>
+    <t>Description:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When searching for a movie that is not in the website database, irrelevant movies are displayed in the search results and there is no message “We are sorry but we do not currently have the movie you are looking for in our collection.”
+</t>
+  </si>
+  <si>
+    <t>Steps to reproduce:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Go to www.testmovies.com
+</t>
+  </si>
+  <si>
+    <t>2.Click on the movie search</t>
+  </si>
+  <si>
+    <t>3.Enter some movie that isn't in the website database</t>
+  </si>
+  <si>
+    <t>4.Click on the button "enter"</t>
+  </si>
+  <si>
+    <t>Actual Result:</t>
+  </si>
+  <si>
+    <t>1.Irrelevant movies are displayed</t>
+  </si>
+  <si>
+    <t>Expected Result:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.The message is displayed “We are sorry but we do not currently have the movie you are looking for in our collection.”
+</t>
+  </si>
+  <si>
+    <t>Attachments:</t>
+  </si>
+  <si>
+    <t>Environment:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windows 7, Google Chrome v. 92.0.4515.107 </t>
+  </si>
+  <si>
+    <t>Components:</t>
+  </si>
+  <si>
+    <t>Movie search</t>
+  </si>
+  <si>
+    <t>Realease:</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>Priority:</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Assignee:</t>
+  </si>
+  <si>
+    <t>Vasily Pupkin</t>
+  </si>
+  <si>
+    <t>Reporter:</t>
+  </si>
+  <si>
+    <t>Alina Paliakova</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,16 +181,43 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6B8AF"/>
+        <bgColor rgb="FFE6B8AF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE5CD"/>
+        <bgColor rgb="FFFCE5CD"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -131,17 +240,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -204,6 +343,50 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4076700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2752725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="image1.jpg"/>
+        <xdr:cNvPicPr preferRelativeResize="0">
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="219075" y="5305425"/>
+          <a:ext cx="3857625" cy="2705100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
@@ -473,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,4 +683,156 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="68.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="108" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="72" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+    </row>
+    <row r="16" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>